<commit_message>
feat: anonimização de dados para doc oficial de marcas
'\sectors\marcas\types\doc_recurso-indef--naoProv\doc_extractor.js'
</commit_message>
<xml_diff>
--- a/Auxiliar/dicionario de Variáveis.xlsx
+++ b/Auxiliar/dicionario de Variáveis.xlsx
@@ -5,14 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Marcas" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Patentes" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Planilha3" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Planilha4" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Marcas!$D$3:$H$65</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Marcas!$B$3:$F$65</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha4!$B$1:$F$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="344">
   <si>
     <t xml:space="preserve">Nome Objeto</t>
   </si>
@@ -323,48 +326,72 @@
     <t xml:space="preserve"> Categoria do documento oficial (valor padrão: documento_oficial). </t>
   </si>
   <si>
+    <t xml:space="preserve"> "documento_oficial",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `tipo`                               </t>
   </si>
   <si>
     <t xml:space="preserve"> Tipo específico do documento.                                     </t>
   </si>
   <si>
+    <t xml:space="preserve"> "recursoIndeferimentoPedidoRegistro_naoProvido",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `subtipo`                            </t>
   </si>
   <si>
     <t xml:space="preserve"> Subtipo do documento.                                             </t>
   </si>
   <si>
+    <t xml:space="preserve"> "",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `confianca`                          </t>
   </si>
   <si>
     <t xml:space="preserve"> Confiança da classificação (0–100).                               </t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.85,</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_numeroProcesso`                </t>
   </si>
   <si>
     <t xml:space="preserve"> Número do processo (9 dígitos).                                   </t>
   </si>
   <si>
+    <t xml:space="preserve"> "929063775",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_dataDespacho`                  </t>
   </si>
   <si>
     <t xml:space="preserve"> Data do despacho (DD/MM/YYYY).                                    </t>
   </si>
   <si>
+    <t xml:space="preserve"> "24/06/2024",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_nomePeticao`                   </t>
   </si>
   <si>
     <t xml:space="preserve"> Nome da petição.                                                  </t>
   </si>
   <si>
+    <t xml:space="preserve"> "Recurso contra indeferimento de pedido de registro de marca (3000.1)",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_numeroProtocolo`               </t>
   </si>
   <si>
     <t xml:space="preserve"> Número do protocolo.                                              </t>
   </si>
   <si>
+    <t xml:space="preserve"> "850240311055",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_dataApresentacao`              </t>
   </si>
   <si>
@@ -377,94 +404,139 @@
     <t xml:space="preserve"> Nome do requerente.                                               </t>
   </si>
   <si>
+    <t xml:space="preserve"> "YOLOVEYO CONFECÇÕES DE PEÇAS DO VESTUARIO LTDA -ME",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_dataNotificacaoIndeferimento`  </t>
   </si>
   <si>
     <t xml:space="preserve"> Data de notificação do indeferimento.                             </t>
   </si>
   <si>
+    <t xml:space="preserve"> "24/04/2024",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_nomeDecisao`                   </t>
   </si>
   <si>
     <t xml:space="preserve"> Nome da decisão.                                                  </t>
   </si>
   <si>
+    <t xml:space="preserve"> "Recurso não provido. Decisão mantida",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_dataParecer`                   </t>
   </si>
   <si>
     <t xml:space="preserve"> Data do parecer.                                                  </t>
   </si>
   <si>
+    <t xml:space="preserve"> "26/01/2026",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_numeroParecer`                 </t>
   </si>
   <si>
     <t xml:space="preserve"> Número do parecer.                                                </t>
   </si>
   <si>
+    <t xml:space="preserve"> "133221",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `textoAutomaticoEtapa1`              </t>
   </si>
   <si>
     <t xml:space="preserve"> Texto automático gerado para a etapa 1.                           </t>
   </si>
   <si>
+    <t xml:space="preserve"> "Processo de registro de marca Processo 929063775 Recurso contra indeferimento de pedido de registro de marca (3000.1) Número de protocolo</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `textoAutomaticoEtapa2`              </t>
   </si>
   <si>
     <t xml:space="preserve"> Texto automático gerado para a etapa 2.                           </t>
   </si>
   <si>
+    <t xml:space="preserve"> "MINISTÉRIO DO DESENVOLVIMENTO, INDÚSTRIA, COMÉRCIO E SERVIÇOS INSTITUTO NACIONAL DA PROPRIEDADE INDUSTRIAL PRESIDÊNCIA Processo de registro de marca Processo 929063775 Recurso contra indeferimento de pedido de registro de marca (3000.1) Número de protocolo</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `textoParecer`                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Texto do parecer.                                                 </t>
   </si>
   <si>
+    <t xml:space="preserve"> "Trata-se de fornecimento de subsídios para a decisão a ser proferida pelo Senhor Presidente do INPI no\nrecurso tempestivamente interposto na forma do art. 212 da Lei n.º 9279/96 – Lei da Propriedade\nIndustrial (LPI), contra ato administrativo proferido pela 1ª instância administrativa.\nPreliminarmente deve ficar consignado que a presente instrução é realizada por meio de consulta direta\naos sistemas informatizados do INPI, no que se refere aos dados das eventuais anterioridades\napontadas, das petições eletrônicas e dos documentos efetivamente digitalizados.\nDiante da análise das argumentações constantes dos autos acerca do ato administrativo recorrido, frente\nao que disciplina as atuais diretrizes de exame definidas no Manual de Marcas em vigor, manifestamo-\nnos nos seguintes termos</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_tecnico`                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Técnico responsável.                                              </t>
   </si>
   <si>
+    <t xml:space="preserve"> "RICARDO FREDERICO NICOL",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `form_marca`                         </t>
   </si>
   <si>
     <t xml:space="preserve"> Marca relacionada ao processo.                                    </t>
   </si>
   <si>
+    <t xml:space="preserve"> "YOLOVEYO",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `tipoDespacho`                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Tipo de despacho (Recurso não provido).                           </t>
   </si>
   <si>
+    <t xml:space="preserve"> "Recurso não provido",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `artigosInvocados`                   </t>
   </si>
   <si>
     <t xml:space="preserve"> Lista de artigos invocados.                                       </t>
   </si>
   <si>
+    <t xml:space="preserve">[         "Art. 124",         "Art. 129"     ],</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `decisao`                            </t>
   </si>
   <si>
     <t xml:space="preserve"> Decisão (indeferido_mantido).                                     </t>
   </si>
   <si>
+    <t xml:space="preserve"> "indeferido_mantido",</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `motivoIndeferimento`                </t>
   </si>
   <si>
     <t xml:space="preserve"> Motivo do indeferimento.                                          </t>
   </si>
   <si>
+    <t xml:space="preserve"> "A marca reproduz ou imita os seguintes registros de terceiros, sendo, portanto, irregistrável de acordo com o inciso XIX do Art. 124 da LPI</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `anterioridades`                     </t>
   </si>
   <si>
     <t xml:space="preserve"> Anterioridades citadas.                                           </t>
   </si>
   <si>
+    <t xml:space="preserve">[         "822293013"     ],</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `processosConflitantes`              </t>
   </si>
   <si>
-    <t xml:space="preserve"> Processos conflitantes citados.                                   </t>
+    <t xml:space="preserve"> Processos conflitantes citados.             Qual a diferença para     `anterioridades`     ?        </t>
   </si>
   <si>
     <t xml:space="preserve"> `textoParaIa`                        </t>
@@ -473,12 +545,18 @@
     <t xml:space="preserve"> Texto do parecer anonimizado para IA.                             </t>
   </si>
   <si>
+    <t xml:space="preserve"> "Trata-se de fornecimento de subsídios para a decisão a ser proferida pelo Senhor Presidente do INPI no\nrecurso tempestivamente interposto na forma do art. 212 da Lei n.º 9279/96 – Lei da Propriedade\nIndustrial (LPI), contra ato administrativo proferido pela 1ª instância administrativa.\napontadas, das petições eletrônicas e dos documentos efetivamente digitalizados.\nDiante da análise das argumentações constantes dos autos acerca do ato administrativo recorrido, frente\nao que disciplina as atuais diretrizes de exame definidas no Manual de Marcas em vigor, manifestamo-\nnos nos seguintes termos</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `textoCompleto`                      </t>
   </si>
   <si>
     <t xml:space="preserve"> Texto completo do documento.                                      </t>
   </si>
   <si>
+    <t xml:space="preserve">    "textoCompleto"</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `urlPdf`                             </t>
   </si>
   <si>
@@ -491,12 +569,24 @@
     <t xml:space="preserve"> Data/hora do processamento.                                       </t>
   </si>
   <si>
+    <t xml:space="preserve"> "2026-02-13T12</t>
+  </si>
+  <si>
     <t xml:space="preserve"> `processor`                          </t>
   </si>
   <si>
     <t xml:space="preserve"> Identificador do processador.                                     </t>
   </si>
   <si>
+    <t xml:space="preserve"> "DocRecursoIndefNaoProvExtractor",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "setor"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "marcas"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Patentes &gt; Petição &gt; Recurso contra Indeferimento de Pedido de Patente </t>
   </si>
   <si>
@@ -717,6 +807,258 @@
   </si>
   <si>
     <t xml:space="preserve"> Identificador do processador. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "categoria"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "tipo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "subtipo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "confianca"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_numeroProcesso"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_dataDespacho"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_nomePeticao"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_numeroProtocolo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_dataApresentacao"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_requerente_nome"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_dataNotificacaoIndeferimento"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_nomeDecisao"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_dataParecer"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_numeroParecer"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "textoAutomaticoEtapa1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 850240311055 Data de apresentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24/06/2024 Requerente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOLOVEYO CONFECÇÕES DE PEÇAS DO VESTUARIO LTDA -ME Indeferimento do pedido Notificada 24/04/2024 Afeta Processo 929063775 (YOLOVEYO) Recurso não provido. Decisão mantida Data do parecer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26/01/2026 Número do parecer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 133221",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "textoAutomaticoEtapa2"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24/06/2024 Situação do recurso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recurso não provido (decisão mantida) Requerente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOLOVEYO CONFECÇÕES DE PEÇAS DO VESTUARIO LTDA -ME Indeferimento do pedido Notificada 24/04/2024 Afeta Processo 929063775 (YOLOVEYO)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "textoParecer"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nPELA MANUTENÇÃO DO ATO INDEFERITÓRIO\nO presente parecer visa fornecer subsídios técnicos ao exame do recurso contra o indeferimento de\npedido de registro de marca, tempestivamente instaurado nos moldes do art. 169 da Lei n.º 9279/96 - Lei\nda Propriedade Industrial (LPI).\nPreliminarmente deve ficar consignado que a presente instrução é realizada por meio de consulta direta\naos sistemas informatizados do INPI, no que se refere aos dados das eventuais anterioridades\napontadas, das petições eletrônicas e dos documentos já digitalizados.\nPROCESSO EM EXAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nProcesso de nº 929063775, depositado em 29/12/2022 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05, marca mista YOLOVEYO, cuja\ntitularidade é de YOLOVEYO CONFECÇÕES DE PEÇAS DO VESTUARIO LTDA -ME / CNPJ\n34091592000116, que foi depositado para distinguir os seguintes produtos e/ou serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35,\ndeferida, comércio (através de qualquer meio) de artigos do vestuário;comércio (através de qualquer\nmeio) de roupas;consultoria em gestão de negócios; Situação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aguardando apresentação ou exame de\nrecurso contra o indeferimento\nFOI INDEFERIDO COM A SEGUINTE MOTIVAÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nA marca reproduz ou imita os seguintes registros de terceiros, sendo, portanto, irregistrável de acordo\ncom o inciso XIX do Art. 124 da LPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Processo 822293013 (YOYO FASHION). Art. 124 - Não são\nregistráveis como marca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XIX - reprodução ou imitação, no todo ou em parte, ainda que com acréscimo,\nde marca alheia registrada, para distinguir ou certificar produto ou serviço idêntico, semelhante ou afim,\nsuscetível de causar confusão ou associação com marca alheia;\nMARCA(S) APONTADA(S) COMO IMPEDITIVA(S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\n1. Processo de nº 822293013, depositado em 31/05/2000 00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00, marca nominativa YOYO\nFASHION, cuja titularidade é de CONFECÇÕES YO YO FAHION LTDA. / CNPJ\n3626375000150, que foi depositado para distinguir os seguintes produtos e/ou serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35,\ndeferida, comercialização de artigos do vestuário e seus acessórios para uso masculino,\nfeminino, infantil e juvenil, a saber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> saias, blusas, vestidos, calças, camisas, camisetas, roupas\nintimas, meias, agasalhos esportivos, malhas de lã, jaquetas, casacos, maios e biquinis,\ncalçados, bonés, cintos.; Situação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Registro de marca em vigor\nInicialmente, informamos que não identificamos o elemento nominativo \" YO\" LOVE\" YO\" na parte\ngráfica ou nominativa da marca, e que está, foi depositada assim, pelos seus responsáveis,\nconforme petição de depósito, ressaltando do parecer de indeferimento \" Cabe observar que a\napresentação mista do sinal em exame destaca os elementos \"YO\" e \"YO\", de modo que o conjunto final\npode ser percebido como a palavra \"YOYO\".\".\nO requerente trouxe os seguintes argumentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\n Não tentou copiar a marca impugnante, fl. 05.\n Fez busca de radical, no sistema web do INPI, fl. 06.\n Preclusão do direito à oposição, de terceiros, fl. 07.\n O conjunto de sua marca, forma um todo indivisível, fl. 09 e fl. 10.\n Que existe suficiente distintividade entre as marcas em confronto, fl. 12.\n suscetível de causar confusão ou associação com marca alheia”,, fl. 13\n Que o logotipo afasta a confusão ou associação entre as marcas em cotejo, fl. 14.\n Que houve a concessão de outras marcas identicas e que deve ser aplicada o princípio da\nisonomia, ao caso, fl. 18.\n Que tem direito à proteção do seu nome empresarial, fl. 21\n Que há ausência de exclusividade de utilização dos elementos nominativos individualmente por\nparte da marca que motivou o indeferimento do pedido de registro de marca da Recorrente, de\nforma que inexistem óbices ao seu registro, fl. 28\n Que tem direito de precedência segundo consta no Art. 129 § 1º da Lei da Propriedade Industrial\nNº. 9.279, de 14/05/96, fl. 28\n Invocando ainda a Política Nacional de Relações de Consumo, fl. 29.\nApós ter sido examinado o ato impugnado e as razões que fundamentaram o recurso, entendemos PELA\nMANUTENÇÃO DO ATO INDEFERITÓRIO, uma vez que o sinal sob exame infringe o disposto no inciso\nXIX do artigo 124 da LPI, na medida em que os sinais em cotejo são semelhantes entre si e se destinam\na assinalar produtos/serviços que guardam afinidade mercadológica, sendo, portanto, suscetíveis de\ncausar confusão ou associação indevida entre eles.\nComo se verifica da figura de busca abaixo, o sinal não está desgastando na classe, por isso, segundo a\nTeoria da Distância, não podem conviver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nQuanto aos demais argumentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\n A defesa com base na \"boa fé\", e na realização de buscas prévias, não são condições\nsuficientes para afastar as impugnações encontradas.\n Sobre à argumentação de defesa com base na preclusão da impugnação no momento\nprocessual da oposição, esta não segue inteligência utilizada no instituto marcário, nem encontra\nrespaldo nos normativos do INPI, pois a oposição é um instrumento facultativo para terceiros,\ncabendo ao INPI, independentemente da existência de oposição, a verificação de ofício da\npossibilidade de impugnação com base nas normas aplicáveis. Além disto, qualquer titular, por\neconomia, pode estar aguardando o prazo previsto no artigo 169 da LPI, caso o INPI não faça o\nindeferimento de ofício, para peticionar um processo administrativo de nulidade.\nLembramos ainda que a Propriedade Industrial não tutela somente os interesses dos titulares,\ncolocando também a sua intenção no interesse social, no desenvolvimento tecnológico e\neconômico do País, e no direito do consumidor.\n Ao caso, não se aplica ateoria do todo indivisível.\n Como demosntrado pela busca, não basta o conjunto ter algum elemento gráfico, para que a\ncolidência seja , de imediato afastada, uma vez que o elemeneto forte da marca é o nominativo.\n Sobre o argumento de defesa com base no nome empresarial, este e a marca são institutos\ndiferentes, por isto são analisados sob critérios distintos, sendo regidos por normas próprias e\nregulados por órgãos diferentes, e cada instituto tem a sua esfera de proteção própria, não\npodendo o argumento ser utilizado como matéria de defesa, no presente caso. Ainda,\nlembramos do art. 129 da LPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nArt. 129. A propriedade da marca adquire-se pelo registro validamente expedido,\nconforme as disposições desta Lei, sendo assegurado ao titular seu uso exclusivo\nem todo o território nacional, observado quanto às marcas coletivas e de\ncertificação o disposto nos arts. 147 e 148. (Grifo Nosso).\n Sobre a \"ausência de exclusividade de utilização dos elementos nominativos\", não trouxe o\nrequerente, argumento convicentes aos autos.\n Afastamos a defesa com base no Art. 129. § 1º, usuário anterior de marca, pois esta somente é\nválida quando há impugnação das anterioridades, em andamento, o qual não é o caso, além\ndisso, não vieram documentos que comprovasse a alegação.\n Os dispositivos constitucionais e consumeristas, fogem ao escopo da presente análise.\nAnte o exposto, submetemos o presente parecer à consideração superior.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_tecnico"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "form_marca"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "tipoDespacho"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "artigosInvocados"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "Art. 124",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "Art. 129"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "decisao"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "motivoIndeferimento"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Processo 822293013 (YOYO FASHION). Art. 124 - Não são registráveis como marca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XIX - reprodução ou imitação, no todo ou em parte, ainda que com acréscimo, de marca alheia registrada, para distinguir ou certificar produto ou serviço idêntico, semelhante ou afim, suscetível de causar confusão ou associação com marca alheia; MARCA(S) APONTADA(S) COMO IMPEDITIVA(S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Processo de nº 822293013, depositado em 31/05/2000 00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00, marca nominativa YOYO FASHION, cuja titularidade é de CONFECÇÕES YO YO FAHION LTDA. / CNPJ 3626375000150, que foi depositado para distinguir os seguintes produtos e/ou serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35, deferida, comercialização de artigos do vestuário e seus acessórios para uso masculino, feminino, infantil e juvenil, a saber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> saias, blusas, vestidos, calças, camisas, camisetas, roupas intimas, meias, agasalhos esportivos, malhas de lã, jaquetas, casacos, maios e biquinis, calçados, bonés, cintos.; Situação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Registro de marca em vigor",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "anterioridades"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "822293013"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "processosConflitantes"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Processo de registro de marca\nProcesso 929063775\nRecurso contra indeferimento de pedido de registro de marca\n(3000.1)\nNúmero de protocolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 850240311055\nData de apresentação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24/06/2024\nRequerente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOLOVEYO CONFECÇÕES DE\nPEÇAS DO VESTUARIO LTDA -ME\nIndeferimento do pedido\nNotificada 24/04/2024 Afeta\nProcesso 929063775\n(YOLOVEYO)\nRecurso não provido. Decisão mantida Data do parecer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26/01/2026\nNúmero do parecer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 133221\nTrata-se de fornecimento de subsídios para a decisão a ser proferida pelo Senhor Presidente do INPI no\nrecurso tempestivamente interposto na forma do art. 212 da Lei n.º 9279/96 – Lei da Propriedade\nIndustrial (LPI), contra ato administrativo proferido pela 1ª instância administrativa.\nPreliminarmente deve ficar consignado que a presente instrução é realizada por meio de consulta direta\naos sistemas informatizados do INPI, no que se refere aos dados das eventuais anterioridades\napontadas, das petições eletrônicas e dos documentos efetivamente digitalizados.\nDiante da análise das argumentações constantes dos autos acerca do ato administrativo recorrido, frente\nao que disciplina as atuais diretrizes de exame definidas no Manual de Marcas em vigor, manifestamo-\nnos nos seguintes termos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nArt. 129. A propriedade da marca adquire-se pelo registro validamente expedido,\nconforme as disposições desta Lei, sendo assegurado ao titular seu uso exclusivo\nem todo o território nacional, observado quanto às marcas coletivas e de\ncertificação o disposto nos arts. 147 e 148. (Grifo Nosso).\n Sobre a \"ausência de exclusividade de utilização dos elementos nominativos\", não trouxe o\nrequerente, argumento convicentes aos autos.\n Afastamos a defesa com base no Art. 129. § 1º, usuário anterior de marca, pois esta somente é\nválida quando há impugnação das anterioridades, em andamento, o qual não é o caso, além\ndisso, não vieram documentos que comprovasse a alegação.\n Os dispositivos constitucionais e consumeristas, fogem ao escopo da presente análise.\nAnte o exposto, submetemos o presente parecer à consideração superior.\nRICARDO FREDERICO NICOL\nDelegação de competência\nPORT/INPI/PR Nº 84/2016\nMINISTÉRIO DO DESENVOLVIMENTO, INDÚSTRIA, COMÉRCIO E SERVIÇOS\nINSTITUTO NACIONAL DA PROPRIEDADE INDUSTRIAL\nPRESIDÊNCIA\nProcesso de registro de marca\nProcesso 929063775\nRecurso contra indeferimento de pedido de registro de marca\n(3000.1)\nNúmero de protocolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24/06/2024\nSituação do recurso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recurso não provido (decisão mantida)\nRequerente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOLOVEYO CONFECÇÕES DE\nPEÇAS DO VESTUARIO LTDA -ME\nIndeferimento do pedido\nNotificada 24/04/2024 Afeta\nProcesso 929063775\n(YOLOVEYO)\nDecisão tomada pelo Presidente\nEm conformidade com o parecer de nº 133221, exarado pela equipe da Coordenação-Geral de Recursos\ne Processos Administrativos de Nulidade – CGREC,\nDECIDO O RECURSO nos termos e condições constantes no referido parecer, ressalvado,\nconforme o caso, a adoção do padrão de apostila instituído por meio da Resolução 166/2016.\nPublique-se a decisão.\nPRESIDENTE DO INPI\n",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "urlPdf"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "dataProcessamento"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.019Z",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "processor"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "textoParaIa"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nPELA MANUTENÇÃO DO ATO INDEFERITÓRIO\nO presente parecer visa fornecer subsídios técnicos ao exame do recurso contra o indeferimento de\npedido de registro de marca, tempestivamente instaurado nos moldes do art. 169 da Lei n.º 9279/96 - Lei\nda Propriedade Industrial (LPI).\napontadas, das petições eletrônicas e dos documentos já digitalizados.\nPROCESSO EM EXAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\nProcesso de nº [PROCESSO_PRINCIPAL_1], depositado em 29/12/2022 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05, marca mista [MARCA_1], cuja\ntitularidade é de [REQUERENTE_1] / CNPJ\n[CNPJ_1], que foi depositado para distinguir os seguintes produtos e/ou serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Processo [PROCESSO_CITADO_1] (YOYO FASHION). Art. 124 - Não são\nregistráveis como marca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\n1. Processo de nº [PROCESSO_CITADO_1], depositado em 31/05/2000 00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">}</t>
   </si>
 </sst>
 </file>
@@ -935,6 +1277,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
@@ -1112,1080 +1458,1092 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D3:I65"/>
+  <dimension ref="B3:F66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E21" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H39" activeCellId="0" sqref="H39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C60" activeCellId="1" sqref="C2:C11 C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="72.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="44.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.62"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="C34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="E39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="4" t="s">
+      <c r="E56" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="4" t="s">
+      <c r="C57" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="4" t="s">
+      <c r="C58" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="4" t="s">
+      <c r="C59" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="4" t="s">
+      <c r="C60" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="C61" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="4" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="4" t="s">
+      <c r="C64" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="4" t="s">
+      <c r="C65" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B66" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
+      <c r="C66" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F66" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="D3:H65"/>
+  <autoFilter ref="B3:F65"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2205,7 +2563,7 @@
   <dimension ref="C2:H68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K48" activeCellId="0" sqref="K48"/>
+      <selection pane="topLeft" activeCell="K48" activeCellId="1" sqref="C2:C11 K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2227,7 +2585,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -2243,7 +2601,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -2252,14 +2610,14 @@
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
@@ -2275,7 +2633,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>16</v>
@@ -2291,23 +2649,23 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>20</v>
@@ -2323,7 +2681,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
@@ -2332,14 +2690,14 @@
         <v>7</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>26</v>
@@ -2355,7 +2713,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>29</v>
@@ -2371,7 +2729,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>32</v>
@@ -2387,7 +2745,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>35</v>
@@ -2403,7 +2761,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>38</v>
@@ -2419,7 +2777,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>41</v>
@@ -2435,7 +2793,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>44</v>
@@ -2451,7 +2809,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>47</v>
@@ -2467,7 +2825,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>50</v>
@@ -2483,23 +2841,23 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>53</v>
@@ -2515,7 +2873,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>56</v>
@@ -2531,7 +2889,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>59</v>
@@ -2547,7 +2905,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>61</v>
@@ -2563,7 +2921,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>63</v>
@@ -2579,7 +2937,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>65</v>
@@ -2595,7 +2953,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>67</v>
@@ -2611,7 +2969,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>69</v>
@@ -2627,7 +2985,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>71</v>
@@ -2643,7 +3001,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>73</v>
@@ -2659,7 +3017,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>78</v>
@@ -2675,7 +3033,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>82</v>
@@ -2684,14 +3042,14 @@
         <v>7</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>85</v>
@@ -2707,7 +3065,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>88</v>
@@ -2723,10 +3081,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
@@ -2739,26 +3097,26 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>7</v>
@@ -2771,480 +3129,480 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>223</v>
+        <v>252</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>224</v>
+        <v>253</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -3259,4 +3617,809 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="E2:AH41"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="1" sqref="C2:C11 E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.94"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="T19" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="U19" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="W19" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y19" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="O35" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="P35" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q35" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="R35" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="T35" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="U35" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="V35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="X35" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y35" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z35" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA35" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB35" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC35" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="AD35" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE35" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="AF35" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG35" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="AH35" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="T39" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="U39" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="V39" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="W39" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="X39" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y39" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:G18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C2:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <autoFilter ref="B1:F11"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: doc oficial de patentes
</commit_message>
<xml_diff>
--- a/Auxiliar/dicionario de Variáveis.xlsx
+++ b/Auxiliar/dicionario de Variáveis.xlsx
@@ -4608,7 +4608,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4635,6 +4635,21 @@
       <b val="true"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF4000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFF4000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -4702,7 +4717,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4731,11 +4746,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4748,7 +4775,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4777,6 +4804,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF4000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -4829,7 +4864,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
@@ -5032,8 +5067,8 @@
   </sheetPr>
   <dimension ref="B3:F66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="1" sqref="B42:B58 C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6134,8 +6169,8 @@
   </sheetPr>
   <dimension ref="A1:CYT67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42:B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18495,7 +18530,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>1349</v>
       </c>
@@ -18512,41 +18547,41 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
+    <row r="54" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
         <v>1349</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="8" t="s">
         <v>1403</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="8" t="s">
         <v>1404</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
+    <row r="55" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
         <v>1349</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="8" t="s">
         <v>1405</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="8" t="s">
         <v>1406</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="8" t="s">
         <v>1402</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
         <v>1349</v>
       </c>
@@ -18597,71 +18632,71 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="59" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
+    <row r="59" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
         <v>1349</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="10" t="s">
         <v>1414</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="10" t="s">
         <v>1416</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="10" t="s">
         <v>1417</v>
       </c>
     </row>
-    <row r="60" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+    <row r="60" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10" t="s">
         <v>1349</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="10" t="s">
         <v>1418</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="10" t="s">
         <v>1419</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="10" t="s">
         <v>1420</v>
       </c>
     </row>
-    <row r="61" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
+    <row r="61" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="s">
         <v>1349</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="10" t="s">
         <v>1421</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="10" t="s">
         <v>1422</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="10" t="s">
         <v>1423</v>
       </c>
     </row>
-    <row r="62" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
+    <row r="62" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10" t="s">
         <v>1349</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="10" t="s">
         <v>1424</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="10" t="s">
         <v>1425</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="10" t="s">
         <v>1423</v>
       </c>
     </row>
@@ -18771,7 +18806,7 @@
   <dimension ref="E2:AH41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+      <selection pane="topLeft" activeCell="E40" activeCellId="1" sqref="B42:B58 E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>